<commit_message>
scanner result change to readonly textarea, change colors, borders
</commit_message>
<xml_diff>
--- a/Page checker/doc/doc.xlsx
+++ b/Page checker/doc/doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="tooltip" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>bower : tracetool.js</t>
   </si>
@@ -33,29 +33,174 @@
     <t>O Specific index</t>
   </si>
   <si>
-    <t>Publish</t>
-  </si>
-  <si>
-    <t>Add a waiting glass (change popup icon ?)</t>
-  </si>
-  <si>
     <t>Array selection : change look : first, last,use cout, specific index</t>
   </si>
   <si>
-    <t>Add import/export button</t>
+    <t>Import/export button</t>
+  </si>
+  <si>
+    <t>If empty list : display overlay help</t>
+  </si>
+  <si>
+    <t>http://www.w3schools.com/bootstrap/bootstrap_tooltip.asp</t>
+  </si>
+  <si>
+    <t>http://www.w3schools.com/css/css_tooltip.asp</t>
+  </si>
+  <si>
+    <t>http://www.w3schools.com/bootstrap/bootstrap_ref_js_tooltip.asp</t>
+  </si>
+  <si>
+    <t>bootstrap</t>
+  </si>
+  <si>
+    <t>http://www.w3schools.com/code/tryit.asp?filename=FCAJCISBK1RZ</t>
+  </si>
+  <si>
+    <t>http://www.nickstakenburg.com/projects/prototip2/</t>
+  </si>
+  <si>
+    <t>http://www.cssportal.com/css-tooltip-generator/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    top    : to move the tooltip on bottom   =&gt; top: 150%;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bottom : to move the tooltip on top      =&gt; bottom:150%;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    */ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    top: 300%;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>&lt;style&gt;</t>
+  </si>
+  <si>
+    <t>.tooltip {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    position: relative;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    display: inline-block;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    border-bottom: 1px dotted black;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>.tooltip .tooltiptext {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    visibility: visible;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    width: 120px;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    background-color: none;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    color: #7cb77f;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    text-align: center;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    border-radius: 6px;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    border-style: solid;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    padding: 5px 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    position: absolute;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    z-index: 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    /* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    position : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    left: 50%;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    margin-left: -60px;</t>
+  </si>
+  <si>
+    <t>.tooltip .tooltiptext::after {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    content: "";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    position :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    top    : to move the tooltip on bottom   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bottom : to move the tooltip on top         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    */</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bottom: 40px;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    margin-left: -30px;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    border-width: 15px;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    /* top,right,bottom,left*/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    border-color: transparent transparent #7cb77f transparent;  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    /*border-color: #7cb77f #7cb77f #7cb77f #7cb77f;  */</t>
+  </si>
+  <si>
+    <t>.tooltip:hover .tooltiptext {</t>
+  </si>
+  <si>
+    <t>&lt;/style&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,14 +235,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -117,34 +268,34 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>191516</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>96038</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>524903</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>86301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5105400" y="180975"/>
-          <a:ext cx="7278116" cy="5649113"/>
+          <a:off x="4743450" y="742950"/>
+          <a:ext cx="7363853" cy="4124901"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -153,6 +304,93 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>264820</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1354430" cy="609599"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangular Callout 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5751220" y="1409700"/>
+          <a:ext cx="1354430" cy="609599"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -31595"/>
+            <a:gd name="adj2" fmla="val -117570"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+            <a:alpha val="91000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-BE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Click</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-BE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> to add  current page to scanner list</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-BE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -199,7 +437,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,10 +469,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,7 +503,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,87 +678,391 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7">
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
       <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="E9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="15.75" thickBot="1">
       <c r="E10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="15.75" thickBot="1">
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7">
       <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B30" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:B58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="63.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try catch on search selector
</commit_message>
<xml_diff>
--- a/Page checker/doc/doc.xlsx
+++ b/Page checker/doc/doc.xlsx
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" activeCellId="1" sqref="B32 B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +774,7 @@
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -806,10 +806,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B30" r:id="rId1"/>
+    <hyperlink ref="B28" r:id="rId2"/>
+    <hyperlink ref="B32" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Selection parsing : InnerHTML, OuterHTML, AllText , MainText
</commit_message>
<xml_diff>
--- a/Page checker/doc/doc.xlsx
+++ b/Page checker/doc/doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,26 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>bower : tracetool.js</t>
   </si>
   <si>
-    <t>O first element</t>
-  </si>
-  <si>
-    <t>O Last element</t>
-  </si>
-  <si>
-    <t>O use count as result</t>
-  </si>
-  <si>
-    <t>O Specific index</t>
-  </si>
-  <si>
-    <t>Array selection : change look : first, last,use cout, specific index</t>
-  </si>
-  <si>
     <t>Import/export button</t>
   </si>
   <si>
@@ -207,23 +192,38 @@
     <t>chrome://extensions/</t>
   </si>
   <si>
-    <t xml:space="preserve">Search result </t>
-  </si>
-  <si>
-    <t>O Inner html</t>
-  </si>
-  <si>
-    <t>O Text without tags</t>
-  </si>
-  <si>
-    <t>O outerHTML</t>
+    <t>http://bitbucket.eortc.be:7990/projects/REG/repos/regulatory/browse?at=refs%2Fheads%2Fbugfix%2FREG-85-users-without-study-template-right</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>http://www.telerik.com/forums/browser-crash-!!-(stack-overflow)</t>
+  </si>
+  <si>
+    <t>.PostTopInfo</t>
+  </si>
+  <si>
+    <t>http://www.telerik.com/forums/how-to-do-data-binding-with-multiple-level-of-functions-calls</t>
+  </si>
+  <si>
+    <t>https://forum.xda-developers.com/xposed/modules/app-fake-wifi-connection-t2800416</t>
+  </si>
+  <si>
+    <t>Move up / down</t>
+  </si>
+  <si>
+    <t>Show last update time</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt; : manage Up and down keys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,12 +237,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -288,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -349,10 +343,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>560095</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>26695</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1354430" cy="609599"/>
     <xdr:sp macro="" textlink="">
@@ -362,7 +356,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7265695" y="1162050"/>
+          <a:off x="7341895" y="1685925"/>
           <a:ext cx="1354430" cy="609599"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
@@ -518,7 +512,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,9 +544,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,6 +579,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -759,109 +755,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="15.75" thickBot="1">
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1">
-      <c r="C11" t="s">
-        <v>4</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="13" spans="2:11">
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11">
-      <c r="C16" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -877,281 +844,281 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
-      <c r="B4" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
-      <c r="B9" t="s">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
-      <c r="B10" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
-      <c r="B12" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
-      <c r="B13" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
-      <c r="B14" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
-      <c r="B15" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
-      <c r="B16" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
-      <c r="B39" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
-      <c r="B46" t="s">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1160,49 +1127,78 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change layout, show last update
</commit_message>
<xml_diff>
--- a/Page checker/doc/doc.xlsx
+++ b/Page checker/doc/doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>bower : tracetool.js</t>
   </si>
@@ -217,13 +217,22 @@
   </si>
   <si>
     <t>&lt;ul&gt; : manage Up and down keys</t>
+  </si>
+  <si>
+    <t>https://www.typescriptlang.org/docs/handbook/declaration-files/introduction.html</t>
+  </si>
+  <si>
+    <t>http://definitelytyped.org/</t>
+  </si>
+  <si>
+    <t>type script declaration file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,7 +521,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,10 +553,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,7 +587,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -755,78 +762,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="K2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="15.75" thickBot="1"/>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1">
       <c r="B11" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
       <c r="B23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2">
       <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2">
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2">
       <c r="B31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2">
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -836,287 +858,289 @@
     <hyperlink ref="B30" r:id="rId1"/>
     <hyperlink ref="B28" r:id="rId2"/>
     <hyperlink ref="B32" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B15" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2">
       <c r="B12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2">
       <c r="B13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2">
       <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2">
       <c r="B16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2">
       <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2">
       <c r="B23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2">
       <c r="B24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2">
       <c r="B26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2">
       <c r="B27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2">
       <c r="B28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2">
       <c r="B30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2">
       <c r="B32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2">
       <c r="B35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2">
       <c r="B36" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2">
       <c r="B37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2">
       <c r="B38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2">
       <c r="B39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2">
       <c r="B40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2">
       <c r="B41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2">
       <c r="B42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2">
       <c r="B43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2">
       <c r="B44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2">
       <c r="B45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2">
       <c r="B46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2">
       <c r="B47" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2">
       <c r="B48" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2">
       <c r="B50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2">
       <c r="B51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2">
       <c r="B52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2">
       <c r="B53" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2">
       <c r="B55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2">
       <c r="B56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2">
       <c r="B57" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2">
       <c r="B58" t="s">
         <v>49</v>
       </c>
@@ -1127,16 +1151,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1144,7 +1168,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1152,7 +1176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1160,7 +1184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1168,7 +1192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1176,12 +1200,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="E8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1189,7 +1213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1197,7 +1221,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="E12" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Move up / down
</commit_message>
<xml_diff>
--- a/Page checker/doc/doc.xlsx
+++ b/Page checker/doc/doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>bower : tracetool.js</t>
   </si>
@@ -210,22 +210,13 @@
     <t>https://forum.xda-developers.com/xposed/modules/app-fake-wifi-connection-t2800416</t>
   </si>
   <si>
-    <t>Move up / down</t>
-  </si>
-  <si>
-    <t>Show last update time</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt; : manage Up and down keys</t>
-  </si>
-  <si>
     <t>https://www.typescriptlang.org/docs/handbook/declaration-files/introduction.html</t>
   </si>
   <si>
     <t>http://definitelytyped.org/</t>
   </si>
   <si>
-    <t>type script declaration file</t>
+    <t>for tracetool : type script declaration file</t>
   </si>
 </sst>
 </file>
@@ -766,7 +757,7 @@
   <dimension ref="B2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -786,36 +777,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-    </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="11" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B11" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B11" s="3"/>
       <c r="G11" s="1"/>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:2">

</xml_diff>